<commit_message>
upload output files to drive
</commit_message>
<xml_diff>
--- a/RPAFinalProject/Data/Config.xlsx
+++ b/RPAFinalProject/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sem5\rpa\final-project\project\RPAFinalProject\RPAFinalProject\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98D68E2-72CF-43F3-8C4E-7C678E24603D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F50B7FE-1798-428E-8A52-D5249CB32215}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{FDE95996-2855-4313-BBCC-E637A92D863D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>path where the charts (as pdfs) will be saved</t>
+  </si>
+  <si>
+    <t>projectFolderID</t>
+  </si>
+  <si>
+    <t>12b1y-sg6E5rox-ntC2UustqiREhdGE5X</t>
+  </si>
+  <si>
+    <t>ID of project ID from Drive</t>
   </si>
 </sst>
 </file>
@@ -439,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C9F770-5B9E-40AD-B46E-53BBC7457D51}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,6 +527,17 @@
         <v>17</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>